<commit_message>
resolve domain related templates
</commit_message>
<xml_diff>
--- a/src/test/resources/com/yqboots/project/initializer/core/workbook.xlsx
+++ b/src/test/resources/com/yqboots/project/initializer/core/workbook.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="203">
   <si>
     <t>URL</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -958,10 +958,6 @@
   </si>
   <si>
     <t>Field Type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Length</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -1671,13 +1667,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.15"/>
@@ -1687,17 +1683,16 @@
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.75" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9" style="1"/>
+    <col min="6" max="6" width="8.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A1" s="11" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B1" s="11" t="s">
         <v>199</v>
@@ -1710,10 +1705,9 @@
       <c r="F1" s="9"/>
       <c r="G1" s="9"/>
       <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="I1" s="10"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="2" t="s">
@@ -1726,22 +1720,19 @@
         <v>201</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>202</v>
+        <v>25</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>28</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="J2" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>197</v>
       </c>
@@ -1757,17 +1748,14 @@
       <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F3" s="1">
-        <v>32</v>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G3" s="1" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -1777,17 +1765,14 @@
       <c r="E4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="1">
-        <v>64</v>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G4" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H4" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1797,17 +1782,14 @@
       <c r="E5" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="1">
-        <v>32</v>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G5" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H5" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1817,17 +1799,14 @@
       <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="1">
-        <v>32</v>
+      <c r="F6" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G6" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>198</v>
       </c>
@@ -1843,17 +1822,14 @@
       <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="1">
-        <v>32</v>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H8" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
@@ -1863,17 +1839,14 @@
       <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F9" s="1">
-        <v>64</v>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G9" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H9" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1883,17 +1856,14 @@
       <c r="E10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="1">
-        <v>32</v>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
       </c>
       <c r="G10" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="H10" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="C11" s="1" t="s">
         <v>42</v>
       </c>
@@ -1903,19 +1873,16 @@
       <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="1">
-        <v>255</v>
+      <c r="F11" s="1" t="b">
+        <v>1</v>
       </c>
       <c r="G11" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="C1:J1"/>
+    <mergeCell ref="C1:I1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>

</xml_diff>